<commit_message>
backend can serve xlsx file
-all associated tests written and passed
</commit_message>
<xml_diff>
--- a/src/main/resources/data/testGroup_1.xlsx
+++ b/src/main/resources/data/testGroup_1.xlsx
@@ -51,19 +51,19 @@
     <t>Jeff</t>
   </si>
   <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>6.3</t>
-  </si>
-  <si>
-    <t>3:02</t>
-  </si>
-  <si>
-    <t>3:27</t>
-  </si>
-  <si>
-    <t>17:58</t>
+    <t>262</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>4:47</t>
+  </si>
+  <si>
+    <t>3:24</t>
+  </si>
+  <si>
+    <t>15:34</t>
   </si>
   <si>
     <t>Jones</t>
@@ -72,16 +72,19 @@
     <t>Timothy</t>
   </si>
   <si>
-    <t>335</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>2:08</t>
-  </si>
-  <si>
-    <t>16:04</t>
+    <t>338</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>2:51</t>
+  </si>
+  <si>
+    <t>3:34</t>
+  </si>
+  <si>
+    <t>15:24</t>
   </si>
   <si>
     <t>Samuels</t>
@@ -90,37 +93,37 @@
     <t>Darnell</t>
   </si>
   <si>
-    <t>288</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>2:32</t>
-  </si>
-  <si>
-    <t>2:17</t>
-  </si>
-  <si>
-    <t>23:53</t>
+    <t>324</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>1:29</t>
+  </si>
+  <si>
+    <t>2:47</t>
+  </si>
+  <si>
+    <t>23:49</t>
   </si>
   <si>
     <t>Fredrick</t>
   </si>
   <si>
-    <t>285</t>
-  </si>
-  <si>
-    <t>5.2</t>
-  </si>
-  <si>
-    <t>3:33</t>
-  </si>
-  <si>
-    <t>1:27</t>
-  </si>
-  <si>
-    <t>13:21</t>
+    <t>276</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>4:50</t>
+  </si>
+  <si>
+    <t>1:38</t>
+  </si>
+  <si>
+    <t>16:50</t>
   </si>
   <si>
     <t>Conway</t>
@@ -129,19 +132,16 @@
     <t>Katherine</t>
   </si>
   <si>
-    <t>243</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>2:18</t>
-  </si>
-  <si>
-    <t>2:38</t>
-  </si>
-  <si>
-    <t>13:46</t>
+    <t>147</t>
+  </si>
+  <si>
+    <t>3:20</t>
+  </si>
+  <si>
+    <t>2:48</t>
+  </si>
+  <si>
+    <t>13:59</t>
   </si>
 </sst>
 </file>
@@ -235,25 +235,25 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>67.0</v>
+        <v>84.0</v>
       </c>
       <c r="E2" t="n">
-        <v>63.0</v>
+        <v>70.0</v>
       </c>
       <c r="F2" t="n">
-        <v>61.0</v>
+        <v>73.0</v>
       </c>
       <c r="G2" t="n">
-        <v>29.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>97.0</v>
+        <v>96.0</v>
       </c>
       <c r="I2" t="n">
-        <v>75.0</v>
+        <v>90.0</v>
       </c>
       <c r="J2" t="n">
-        <v>392.0</v>
+        <v>413.0</v>
       </c>
     </row>
     <row r="3">
@@ -270,22 +270,22 @@
         <v>99.0</v>
       </c>
       <c r="E3" t="n">
-        <v>4.0</v>
+        <v>100.0</v>
       </c>
       <c r="F3" t="n">
-        <v>99.0</v>
+        <v>100.0</v>
       </c>
       <c r="G3" t="n">
-        <v>26.0</v>
+        <v>37.0</v>
       </c>
       <c r="H3" t="n">
-        <v>71.0</v>
+        <v>98.0</v>
       </c>
       <c r="I3" t="n">
-        <v>86.0</v>
+        <v>90.0</v>
       </c>
       <c r="J3" t="n">
-        <v>385.0</v>
+        <v>524.0</v>
       </c>
     </row>
     <row r="4">
@@ -293,31 +293,31 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>90.0</v>
+        <v>96.0</v>
       </c>
       <c r="E4" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="G4" t="n">
         <v>100.0</v>
       </c>
-      <c r="F4" t="n">
-        <v>89.0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>56.0</v>
-      </c>
       <c r="H4" t="n">
-        <v>74.0</v>
+        <v>83.0</v>
       </c>
       <c r="I4" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="J4" t="n">
-        <v>412.0</v>
+        <v>469.0</v>
       </c>
     </row>
     <row r="5">
@@ -328,28 +328,28 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="n">
-        <v>87.0</v>
+        <v>85.0</v>
       </c>
       <c r="E5" t="n">
-        <v>52.0</v>
+        <v>66.0</v>
       </c>
       <c r="F5" t="n">
-        <v>88.0</v>
+        <v>63.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>62.0</v>
+        <v>65.0</v>
       </c>
       <c r="I5" t="n">
-        <v>100.0</v>
+        <v>82.0</v>
       </c>
       <c r="J5" t="n">
-        <v>389.0</v>
+        <v>361.0</v>
       </c>
     </row>
     <row r="6">
@@ -357,31 +357,31 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="E6" t="n">
         <v>100.0</v>
       </c>
-      <c r="E6" t="n">
-        <v>60.0</v>
-      </c>
       <c r="F6" t="n">
-        <v>98.0</v>
+        <v>68.0</v>
       </c>
       <c r="G6" t="n">
-        <v>88.0</v>
+        <v>55.0</v>
       </c>
       <c r="H6" t="n">
-        <v>82.0</v>
+        <v>85.0</v>
       </c>
       <c r="I6" t="n">
         <v>100.0</v>
       </c>
       <c r="J6" t="n">
-        <v>528.0</v>
+        <v>479.0</v>
       </c>
     </row>
   </sheetData>
@@ -476,13 +476,13 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -490,28 +490,28 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -522,25 +522,25 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
@@ -548,19 +548,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>40</v>

</xml_diff>